<commit_message>
modified adversarial training method
</commit_message>
<xml_diff>
--- a/demo_mnist/adversarial_training/result.xlsx
+++ b/demo_mnist/adversarial_training/result.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94941401-BA61-46FE-A18E-9D9ED0619B8B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35611A71-847E-43A8-9220-68246A2EA374}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>LAT_model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,7 +122,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>改进版对抗训练模型(alpha = 0.5,std = 0.2)</t>
+    <t>改进版对抗训练模型(alpha = 0.5,std = 0.2,,method = 'fgsm')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>改进版对抗训练模型(alpha = 0.5,std = 0.2,,method = 'tfgsm')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fgsm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ifgsm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ε=0.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hyperparameters</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -130,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +166,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -173,9 +210,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -456,215 +498,318 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="54.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>0.97</v>
-      </c>
-      <c r="C2">
+      <c r="B5">
+        <v>0.97</v>
+      </c>
+      <c r="C5">
         <v>0.99</v>
       </c>
-      <c r="D2">
-        <v>0.97</v>
-      </c>
-      <c r="E2">
-        <v>0.97</v>
-      </c>
-      <c r="F2">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D5">
+        <v>0.97</v>
+      </c>
+      <c r="E5">
+        <v>0.97</v>
+      </c>
+      <c r="F5">
+        <v>0.97</v>
+      </c>
+      <c r="G5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B6">
         <v>0.72</v>
       </c>
-      <c r="C3">
-        <v>0.97</v>
-      </c>
-      <c r="D3">
-        <v>0.97</v>
-      </c>
-      <c r="E3">
+      <c r="C6">
+        <v>0.97</v>
+      </c>
+      <c r="D6">
+        <v>0.97</v>
+      </c>
+      <c r="E6">
         <v>0.96</v>
       </c>
-      <c r="F3">
+      <c r="F6">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="G6">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C4">
+      <c r="C7">
         <v>0.92</v>
       </c>
-      <c r="D4">
-        <v>0.97</v>
-      </c>
-      <c r="E4">
+      <c r="D7">
+        <v>0.97</v>
+      </c>
+      <c r="E7">
         <v>0.92</v>
       </c>
-      <c r="F4">
+      <c r="F7">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="G7">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>0.04</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>0.73</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <v>0.95</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>0.78</v>
       </c>
-      <c r="F5">
+      <c r="F8">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.97</v>
+      </c>
+      <c r="D11">
+        <v>0.97</v>
+      </c>
+      <c r="E11">
+        <v>0.96</v>
+      </c>
+      <c r="F11">
+        <v>0.94</v>
+      </c>
+      <c r="G11">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>0.15</v>
+      </c>
+      <c r="C12">
+        <v>0.95</v>
+      </c>
+      <c r="D12">
+        <v>0.96</v>
+      </c>
+      <c r="E12">
+        <v>0.94</v>
+      </c>
+      <c r="F12">
+        <v>0.92</v>
+      </c>
+      <c r="G12">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>0.01</v>
+      </c>
+      <c r="C13">
+        <v>0.91</v>
+      </c>
+      <c r="D13">
+        <v>0.95</v>
+      </c>
+      <c r="E13">
+        <v>0.92</v>
+      </c>
+      <c r="F13">
+        <v>0.88</v>
+      </c>
+      <c r="G13">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B20" t="b">
+      <c r="B20" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" t="b">
+      <c r="B23" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new LAT testing result of MNIST
</commit_message>
<xml_diff>
--- a/demo_mnist/adversarial_training/result.xlsx
+++ b/demo_mnist/adversarial_training/result.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35611A71-847E-43A8-9220-68246A2EA374}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C490CF3D-34A0-402C-8628-FB180D71EBAC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>LAT_model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,10 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>逐层对抗训练模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>传统对抗训练模型(eps=0.2,alpha = 0.5)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,6 +139,18 @@
   </si>
   <si>
     <t>hyperparameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逐层对抗训练模型(change the bp method,without ZeroReg)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逐层对抗训练模型(change the bp method,ZeroReg every steps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始逐层对抗训练模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,22 +506,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="38.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="54.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="59.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -533,8 +545,15 @@
       <c r="G1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -542,27 +561,34 @@
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -584,8 +610,14 @@
       <c r="G5">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>0.99</v>
+      </c>
+      <c r="I5">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,8 +639,14 @@
       <c r="G6">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>0.97</v>
+      </c>
+      <c r="I6">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,8 +668,14 @@
       <c r="G7">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>0.93</v>
+      </c>
+      <c r="I7">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -653,13 +697,19 @@
       <c r="G8">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>0.76</v>
+      </c>
+      <c r="I8">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,9 +732,9 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>0.15</v>
@@ -705,7 +755,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -728,12 +778,12 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -741,7 +791,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -749,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -757,7 +807,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -765,7 +815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -773,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -781,7 +831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -789,7 +839,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -797,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -805,7 +855,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
add new LAT training method testing result in demo_mnist/adversarial_training
</commit_message>
<xml_diff>
--- a/demo_mnist/adversarial_training/result.xlsx
+++ b/demo_mnist/adversarial_training/result.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C490CF3D-34A0-402C-8628-FB180D71EBAC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3157602C-734F-489E-9B3D-6181DDF2FB58}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>LAT_model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,14 @@
   </si>
   <si>
     <t>原始逐层对抗训练模型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逐层对抗训练模型(fgsm.eps = 0.3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逐层对抗训练模型(change the bp method and fp method)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -506,26 +514,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="63.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="59.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="54.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="59.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -551,9 +559,14 @@
       <c r="I1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -581,14 +594,19 @@
       <c r="I2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -616,8 +634,14 @@
       <c r="I5">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0.96</v>
+      </c>
+      <c r="K5">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -645,8 +669,14 @@
       <c r="I6">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0.92</v>
+      </c>
+      <c r="K6">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -674,8 +704,14 @@
       <c r="I7">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0.84</v>
+      </c>
+      <c r="K7">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -703,13 +739,19 @@
       <c r="I8">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0.69</v>
+      </c>
+      <c r="K8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -732,7 +774,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -755,7 +797,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -778,12 +820,12 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -791,7 +833,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -799,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -807,7 +849,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -815,7 +857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -823,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -831,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -839,7 +881,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -847,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -855,7 +897,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>16</v>
       </c>

</xml_diff>